<commit_message>
fixing Mercina's reply mail
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
   <si>
     <t>KOFCOL TRB SFA</t>
   </si>
@@ -51,9 +51,6 @@
     <t>ITEfactor</t>
   </si>
   <si>
-    <t>KOFCOL TRB CKE</t>
-  </si>
-  <si>
     <t>N194322</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>CH</t>
   </si>
   <si>
-    <t>52927.36f</t>
-  </si>
-  <si>
     <t>1.5f</t>
   </si>
   <si>
@@ -202,6 +196,9 @@
   </si>
   <si>
     <t>Automation_CKEHydromod</t>
+  </si>
+  <si>
+    <t>KOFCOL TRB CKQ</t>
   </si>
 </sst>
 </file>
@@ -634,57 +631,57 @@
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -696,7 +693,7 @@
         <v>10503512</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>1</v>
@@ -708,25 +705,25 @@
         <v>3</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P2" s="3">
         <v>22</v>
@@ -796,60 +793,60 @@
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4">
         <v>1813</v>
@@ -858,37 +855,37 @@
         <v>30493722</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I2" s="4">
         <v>13012004</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P2" s="3">
         <v>22</v>
@@ -928,7 +925,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -956,69 +955,69 @@
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="C2" s="4">
         <v>1723</v>
@@ -1027,16 +1026,16 @@
         <v>20291426</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I2" s="4">
         <v>2</v>
@@ -1045,28 +1044,28 @@
         <v>1</v>
       </c>
       <c r="K2" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="S2" s="3">
         <v>22</v>
@@ -1123,30 +1122,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1191,53 +1190,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2">
         <v>1713</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>1723</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
including changes done for multiequipment
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\con_svijay02\KTOC-TRB-Automation\KTOC_TRB_TestAutomation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\con_svijay02\KTOC-TRB-Automation\KTOC_TRB_TestMethods\src\com\KTOC\TRB\testautomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="France" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="75">
   <si>
     <t>KOFCOL TRB SFA</t>
   </si>
@@ -48,6 +48,9 @@
     <t>Automation_Template_002</t>
   </si>
   <si>
+    <t>Discount</t>
+  </si>
+  <si>
     <t>ITEfactor</t>
   </si>
   <si>
@@ -84,6 +87,18 @@
     <t>TemplateName</t>
   </si>
   <si>
+    <t>withoutFirstMaintenance</t>
+  </si>
+  <si>
+    <t>withFirstMaintenance1</t>
+  </si>
+  <si>
+    <t>withFirstMaintenance2</t>
+  </si>
+  <si>
+    <t>TenderPrice</t>
+  </si>
+  <si>
     <t>RegionalDiscount</t>
   </si>
   <si>
@@ -192,13 +207,52 @@
     <t>s.vijay@kone.com.qa</t>
   </si>
   <si>
-    <t>2.47f</t>
+    <t>KOFCOL TRB CKQ</t>
   </si>
   <si>
     <t>Automation_CKEHydromod</t>
   </si>
   <si>
-    <t>KOFCOL TRB CKQ</t>
+    <t>EquipmentID_2</t>
+  </si>
+  <si>
+    <t>TemplateName2</t>
+  </si>
+  <si>
+    <t>Automation_Template_forEscalator</t>
+  </si>
+  <si>
+    <t>GroupName</t>
+  </si>
+  <si>
+    <t>Automation_GroupName</t>
+  </si>
+  <si>
+    <t>EquipmentinService_Escalator</t>
+  </si>
+  <si>
+    <t>EIS Escalator</t>
+  </si>
+  <si>
+    <t>4f</t>
+  </si>
+  <si>
+    <t>changeRegionalDiscount</t>
+  </si>
+  <si>
+    <t>changeITEfactor</t>
+  </si>
+  <si>
+    <t>2.75f</t>
+  </si>
+  <si>
+    <t>-5f</t>
+  </si>
+  <si>
+    <t>changeSupervisor</t>
+  </si>
+  <si>
+    <t>06151495</t>
   </si>
 </sst>
 </file>
@@ -270,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -290,6 +344,13 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,9 +665,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -614,74 +675,122 @@
     <col min="2" max="2" width="13.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.7265625" style="5"/>
+    <col min="5" max="5" width="11.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.08984375" style="5" customWidth="1"/>
+    <col min="17" max="17" width="18.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.6328125" style="11" customWidth="1"/>
+    <col min="20" max="20" width="6.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>36</v>
+      <c r="U1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -692,40 +801,76 @@
       <c r="D2" s="4">
         <v>10503512</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>29</v>
+      <c r="E2" s="4">
+        <v>11234846</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="J2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="O2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P2" s="3">
+        <v>63</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>0</v>
+      </c>
+      <c r="R2" s="10">
+        <v>3</v>
+      </c>
+      <c r="S2" s="10">
+        <v>6</v>
+      </c>
+      <c r="T2" s="10">
+        <v>10</v>
+      </c>
+      <c r="U2" s="10">
+        <v>2001</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" s="3">
         <v>22</v>
       </c>
     </row>
@@ -733,7 +878,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I2" numberStoredAsText="1"/>
+    <ignoredError sqref="J2:K2" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -754,7 +899,7 @@
           <x14:formula1>
             <xm:f>'-na-'!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E2</xm:sqref>
+          <xm:sqref>F2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -764,10 +909,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -783,70 +928,89 @@
     <col min="9" max="9" width="8.08984375" style="5" customWidth="1"/>
     <col min="10" max="10" width="14.6328125" style="5" customWidth="1"/>
     <col min="11" max="11" width="22.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7265625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="7" style="5" customWidth="1"/>
-    <col min="14" max="14" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.7265625" style="5"/>
+    <col min="12" max="12" width="18.26953125" style="5" customWidth="1"/>
+    <col min="13" max="14" width="16.6328125" style="5" customWidth="1"/>
+    <col min="15" max="15" width="6.81640625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="9" style="5" customWidth="1"/>
+    <col min="17" max="17" width="12.7265625" style="5" customWidth="1"/>
+    <col min="18" max="18" width="7" style="5" customWidth="1"/>
+    <col min="19" max="19" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C2" s="4">
         <v>1813</v>
@@ -855,39 +1019,54 @@
         <v>30493722</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="I2" s="4">
         <v>13012004</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>3</v>
+      </c>
+      <c r="N2" s="4">
+        <v>6</v>
+      </c>
+      <c r="O2" s="4">
+        <v>10</v>
+      </c>
+      <c r="P2" s="4">
+        <v>2001</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="P2" s="3">
+      <c r="S2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" s="3">
         <v>22</v>
       </c>
     </row>
@@ -923,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -945,79 +1124,98 @@
     <col min="12" max="12" width="8.08984375" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.6328125" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.7265625" style="5"/>
+    <col min="15" max="15" width="18.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="16.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C2" s="4">
         <v>1723</v>
@@ -1026,16 +1224,16 @@
         <v>20291426</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="I2" s="4">
         <v>2</v>
@@ -1047,27 +1245,42 @@
         <v>1</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O2" s="4">
+        <v>0</v>
+      </c>
+      <c r="P2" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>6</v>
+      </c>
+      <c r="R2" s="4">
+        <v>10</v>
+      </c>
+      <c r="S2" s="4">
+        <v>2001</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" s="3">
+      <c r="V2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" s="3">
         <v>22</v>
       </c>
     </row>
@@ -1109,7 +1322,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1122,37 +1335,37 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'-na-'!$B$2:$B$3</xm:f>
@@ -1190,53 +1403,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>1713</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>1723</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
including labourrate in testdata
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\con_svijay02\KTOC-TRB-Automation\KTOC_TRB_TestMethods\src\com\KTOC\TRB\testautomation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\con_svijay02\KTOC-TRB-Automation\KTOC_TRB_TestAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="79">
   <si>
     <t>KOFCOL TRB SFA</t>
   </si>
@@ -253,6 +253,18 @@
   </si>
   <si>
     <t>06151495</t>
+  </si>
+  <si>
+    <t>LabourRate</t>
+  </si>
+  <si>
+    <t>61.9</t>
+  </si>
+  <si>
+    <t>changeLabourRate</t>
+  </si>
+  <si>
+    <t>61</t>
   </si>
 </sst>
 </file>
@@ -665,7 +677,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -696,13 +708,15 @@
     <col min="23" max="23" width="17.90625" style="5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" style="5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="8.7265625" style="5"/>
+    <col min="26" max="26" width="12" style="5" customWidth="1"/>
+    <col min="27" max="27" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -779,16 +793,22 @@
         <v>70</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -864,13 +884,19 @@
       <c r="Y2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AD2" s="3">
         <v>22</v>
       </c>
     </row>
@@ -878,7 +904,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J2:K2" numberStoredAsText="1"/>
+    <ignoredError sqref="J2:K2 Z2:AA2" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>

<commit_message>
updating method for multiequipment
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="France" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="88">
   <si>
     <t>KOFCOL TRB SFA</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>88</t>
+  </si>
+  <si>
+    <t>13010164</t>
+  </si>
+  <si>
+    <t>07003009</t>
   </si>
 </sst>
 </file>
@@ -700,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -958,7 +964,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A1:AD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1113,11 +1121,11 @@
       <c r="I2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>47</v>
+      <c r="J2" s="4">
+        <v>13012004</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>9</v>
@@ -1181,7 +1189,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J2:K2 Z2" numberStoredAsText="1"/>
+    <ignoredError sqref="Z2:AA2 K2" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1214,7 +1222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1366,7 +1374,7 @@
         <v>20291426</v>
       </c>
       <c r="E2" s="4">
-        <v>11234846</v>
+        <v>20291427</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>34</v>
@@ -1393,7 +1401,7 @@
         <v>52</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
removing HydraulicElevCheck for multiequipment
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="France" sheetId="7" r:id="rId1"/>
@@ -706,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1222,7 +1222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
including data retriving from fullgrid
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -234,9 +234,6 @@
     <t>EIS Escalator</t>
   </si>
   <si>
-    <t>4f</t>
-  </si>
-  <si>
     <t>changeRegionalDiscount</t>
   </si>
   <si>
@@ -292,6 +289,9 @@
   </si>
   <si>
     <t>07003009</t>
+  </si>
+  <si>
+    <t>4.18f</t>
   </si>
 </sst>
 </file>
@@ -706,7 +706,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -775,7 +777,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>17</v>
@@ -811,19 +813,19 @@
         <v>23</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>39</v>
@@ -867,7 +869,7 @@
         <v>47</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>9</v>
@@ -900,22 +902,22 @@
         <v>2001</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="X2" s="8" t="s">
         <v>46</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Z2" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AA2" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB2" s="3" t="s">
         <v>43</v>
@@ -1033,7 +1035,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>17</v>
@@ -1069,19 +1071,19 @@
         <v>23</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>39</v>
@@ -1125,7 +1127,7 @@
         <v>13012004</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>9</v>
@@ -1158,22 +1160,22 @@
         <v>2001</v>
       </c>
       <c r="V2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="X2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="Z2" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="AA2" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="AB2" s="3" t="s">
         <v>43</v>
@@ -1300,7 +1302,7 @@
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>17</v>
@@ -1336,19 +1338,19 @@
         <v>23</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>39</v>
@@ -1401,7 +1403,7 @@
         <v>52</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>9</v>
@@ -1437,19 +1439,19 @@
         <v>45</v>
       </c>
       <c r="Z2" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AA2" s="8" t="s">
         <v>38</v>
       </c>
       <c r="AB2" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AC2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD2" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="AD2" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
fixed assert in RegionalDiscount & DetailBreakdownTab
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
   <si>
     <t>KOFCOL TRB SFA</t>
   </si>
@@ -240,12 +240,6 @@
     <t>changeITEfactor</t>
   </si>
   <si>
-    <t>2.75f</t>
-  </si>
-  <si>
-    <t>-5f</t>
-  </si>
-  <si>
     <t>changeSupervisor</t>
   </si>
   <si>
@@ -292,6 +286,9 @@
   </si>
   <si>
     <t>4.18f</t>
+  </si>
+  <si>
+    <t>-3.34f</t>
   </si>
 </sst>
 </file>
@@ -706,9 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -777,7 +772,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>17</v>
@@ -822,10 +817,10 @@
         <v>69</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>39</v>
@@ -869,7 +864,7 @@
         <v>47</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>9</v>
@@ -902,22 +897,22 @@
         <v>2001</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="X2" s="8" t="s">
         <v>46</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="Z2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA2" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>77</v>
       </c>
       <c r="AB2" s="3" t="s">
         <v>43</v>
@@ -1035,7 +1030,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>17</v>
@@ -1080,10 +1075,10 @@
         <v>69</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>39</v>
@@ -1127,7 +1122,7 @@
         <v>13012004</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>9</v>
@@ -1160,22 +1155,22 @@
         <v>2001</v>
       </c>
       <c r="V2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z2" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="AA2" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="Y2" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="AB2" s="3" t="s">
         <v>43</v>
@@ -1302,7 +1297,7 @@
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>17</v>
@@ -1347,10 +1342,10 @@
         <v>69</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>39</v>
@@ -1403,7 +1398,7 @@
         <v>52</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>9</v>
@@ -1439,19 +1434,19 @@
         <v>45</v>
       </c>
       <c r="Z2" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AA2" s="8" t="s">
         <v>38</v>
       </c>
       <c r="AB2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="AC2" s="8" t="s">
-        <v>83</v>
-      </c>
       <c r="AD2" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
including condition for +0.02
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="97">
   <si>
     <t>KOFCOL TRB SFA</t>
   </si>
@@ -285,10 +285,40 @@
     <t>07003009</t>
   </si>
   <si>
-    <t>4.18f</t>
-  </si>
-  <si>
-    <t>-3.34f</t>
+    <t>-4f</t>
+  </si>
+  <si>
+    <t>RegionalDiscount_MultipleEqup</t>
+  </si>
+  <si>
+    <t>changeRegionalDiscount_MultipleEqup</t>
+  </si>
+  <si>
+    <t>4f</t>
+  </si>
+  <si>
+    <t>-5f</t>
+  </si>
+  <si>
+    <t>ITEfactor_MultipleEqup</t>
+  </si>
+  <si>
+    <t>changeITEfactor_MultipleEqup</t>
+  </si>
+  <si>
+    <t>LabourRate_MultipleEqup</t>
+  </si>
+  <si>
+    <t>changeLabourRate__MultipleEqup</t>
+  </si>
+  <si>
+    <t>2.75f</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>56</t>
   </si>
 </sst>
 </file>
@@ -701,9 +731,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
@@ -730,17 +762,22 @@
     <col min="21" max="21" width="9" style="11" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12" style="5" customWidth="1"/>
-    <col min="27" max="27" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="8.7265625" style="5"/>
+    <col min="24" max="24" width="23.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7" style="5" customWidth="1"/>
+    <col min="29" max="30" width="12" style="5" customWidth="1"/>
+    <col min="31" max="31" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="24.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -811,28 +848,46 @@
         <v>68</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -897,30 +952,48 @@
         <v>2001</v>
       </c>
       <c r="V2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="W2" s="8" t="s">
-        <v>86</v>
-      </c>
       <c r="X2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="AA2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="AC2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD2" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="AA2" s="8" t="s">
+      <c r="AE2" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AF2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AG2" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AD2" s="3">
+      <c r="AJ2" s="3">
         <v>22</v>
       </c>
     </row>
@@ -928,11 +1001,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J2:K2 Z2:AA2" numberStoredAsText="1"/>
+    <ignoredError sqref="J2:K2 AD2:AF2 AG2" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'-na-'!$C$2:$C$3</xm:f>

</xml_diff>

<commit_message>
fixing canada on verifyTargetPriceDisplayedCorrectly
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="France" sheetId="7" r:id="rId1"/>
@@ -733,7 +733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+    <sheetView topLeftCell="Y1" workbookViewId="0">
       <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
@@ -1568,7 +1568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
partially updating actionitem_1 Entering 'First Maintenance' value if not available for Canada
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="France" sheetId="7" r:id="rId1"/>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="97">
-  <si>
-    <t>KOFCOL TRB SFA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="101">
   <si>
     <t>A10137873</t>
   </si>
@@ -45,9 +42,6 @@
     <t>Supervisor</t>
   </si>
   <si>
-    <t>Automation_Template_002</t>
-  </si>
-  <si>
     <t>Discount</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     <t>CH</t>
   </si>
   <si>
-    <t>1.5f</t>
-  </si>
-  <si>
     <t>StageProbabilityStage</t>
   </si>
   <si>
@@ -165,167 +156,188 @@
     <t>Automation Test Description</t>
   </si>
   <si>
-    <t>5f</t>
-  </si>
-  <si>
-    <t>2f</t>
-  </si>
-  <si>
     <t>06114080</t>
   </si>
   <si>
-    <t>KOFCOL TRB 201</t>
-  </si>
-  <si>
     <t>AU21 - Sydney Region</t>
   </si>
   <si>
     <t>AU22 - Newcastle Region</t>
   </si>
   <si>
+    <t>07006025</t>
+  </si>
+  <si>
+    <t>Montréal</t>
+  </si>
+  <si>
+    <t>Québec City</t>
+  </si>
+  <si>
+    <t>SeismicArea</t>
+  </si>
+  <si>
+    <t>WeeklyTeamCostforZone</t>
+  </si>
+  <si>
+    <t>WeeklyTeamCostforRoomandBoard</t>
+  </si>
+  <si>
+    <t>EquipmentID_2</t>
+  </si>
+  <si>
+    <t>TemplateName2</t>
+  </si>
+  <si>
+    <t>Automation_Template_forEscalator</t>
+  </si>
+  <si>
+    <t>GroupName</t>
+  </si>
+  <si>
+    <t>Automation_GroupName</t>
+  </si>
+  <si>
+    <t>EquipmentinService_Escalator</t>
+  </si>
+  <si>
+    <t>EIS Escalator</t>
+  </si>
+  <si>
+    <t>changeRegionalDiscount</t>
+  </si>
+  <si>
+    <t>changeITEfactor</t>
+  </si>
+  <si>
+    <t>changeSupervisor</t>
+  </si>
+  <si>
+    <t>06151495</t>
+  </si>
+  <si>
+    <t>LabourRate</t>
+  </si>
+  <si>
+    <t>changeLabourRate</t>
+  </si>
+  <si>
+    <t>0f</t>
+  </si>
+  <si>
+    <t>2.47f</t>
+  </si>
+  <si>
+    <t>73.68</t>
+  </si>
+  <si>
+    <t>13010164</t>
+  </si>
+  <si>
+    <t>07003009</t>
+  </si>
+  <si>
+    <t>RegionalDiscount_MultipleEqup</t>
+  </si>
+  <si>
+    <t>changeRegionalDiscount_MultipleEqup</t>
+  </si>
+  <si>
+    <t>ITEfactor_MultipleEqup</t>
+  </si>
+  <si>
+    <t>changeITEfactor_MultipleEqup</t>
+  </si>
+  <si>
+    <t>LabourRate_MultipleEqup</t>
+  </si>
+  <si>
+    <t>changeLabourRate__MultipleEqup</t>
+  </si>
+  <si>
+    <t>AUTOMATION TRB SFA</t>
+  </si>
+  <si>
+    <t>s.vijay@kone.com.qap</t>
+  </si>
+  <si>
     <t>AustraliaRopes_For Automation</t>
   </si>
   <si>
-    <t>07006025</t>
-  </si>
-  <si>
-    <t>Montréal</t>
-  </si>
-  <si>
-    <t>Québec City</t>
-  </si>
-  <si>
-    <t>SeismicArea</t>
-  </si>
-  <si>
-    <t>WeeklyTeamCostforZone</t>
-  </si>
-  <si>
-    <t>WeeklyTeamCostforRoomandBoard</t>
-  </si>
-  <si>
-    <t>s.vijay@kone.com.qa</t>
-  </si>
-  <si>
-    <t>KOFCOL TRB CKQ</t>
-  </si>
-  <si>
-    <t>Automation_CKEHydromod</t>
-  </si>
-  <si>
-    <t>EquipmentID_2</t>
-  </si>
-  <si>
-    <t>TemplateName2</t>
-  </si>
-  <si>
-    <t>Automation_Template_forEscalator</t>
-  </si>
-  <si>
-    <t>GroupName</t>
-  </si>
-  <si>
-    <t>Automation_GroupName</t>
-  </si>
-  <si>
-    <t>EquipmentinService_Escalator</t>
-  </si>
-  <si>
-    <t>EIS Escalator</t>
-  </si>
-  <si>
-    <t>changeRegionalDiscount</t>
-  </si>
-  <si>
-    <t>changeITEfactor</t>
-  </si>
-  <si>
-    <t>changeSupervisor</t>
-  </si>
-  <si>
-    <t>06151495</t>
-  </si>
-  <si>
-    <t>LabourRate</t>
-  </si>
-  <si>
-    <t>61.9</t>
-  </si>
-  <si>
-    <t>changeLabourRate</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>0f</t>
-  </si>
-  <si>
-    <t>2.47f</t>
-  </si>
-  <si>
-    <t>73.68</t>
-  </si>
-  <si>
-    <t>1.75f</t>
-  </si>
-  <si>
-    <t>6.7f</t>
-  </si>
-  <si>
-    <t>87.42</t>
-  </si>
-  <si>
-    <t>88</t>
-  </si>
-  <si>
-    <t>13010164</t>
-  </si>
-  <si>
-    <t>07003009</t>
-  </si>
-  <si>
-    <t>-4f</t>
-  </si>
-  <si>
-    <t>RegionalDiscount_MultipleEqup</t>
-  </si>
-  <si>
-    <t>changeRegionalDiscount_MultipleEqup</t>
-  </si>
-  <si>
-    <t>4f</t>
-  </si>
-  <si>
-    <t>-5f</t>
-  </si>
-  <si>
-    <t>ITEfactor_MultipleEqup</t>
-  </si>
-  <si>
-    <t>changeITEfactor_MultipleEqup</t>
-  </si>
-  <si>
-    <t>LabourRate_MultipleEqup</t>
-  </si>
-  <si>
-    <t>changeLabourRate__MultipleEqup</t>
-  </si>
-  <si>
-    <t>2.75f</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>56</t>
+    <t>AutomationSFA</t>
+  </si>
+  <si>
+    <t>0.92f</t>
+  </si>
+  <si>
+    <t>59.1</t>
+  </si>
+  <si>
+    <t>1f</t>
+  </si>
+  <si>
+    <t>95.48</t>
+  </si>
+  <si>
+    <t>Sherbrooke</t>
+  </si>
+  <si>
+    <t>SalesOffice_Canada</t>
+  </si>
+  <si>
+    <t>AUTOMATION TRB CKQ</t>
+  </si>
+  <si>
+    <t>AUTOMATION TRB 201</t>
+  </si>
+  <si>
+    <t>AutomationCKQ</t>
+  </si>
+  <si>
+    <t>84.87</t>
+  </si>
+  <si>
+    <t>isFirstMaintenancetoEdit</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>isFirstMaintenancetoEdittoChange_1</t>
+  </si>
+  <si>
+    <t>isFirstMaintenancetoEdittoChange_2</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>185</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,6 +355,13 @@
     </font>
     <font>
       <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -403,7 +422,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -417,6 +435,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,16 +750,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.453125" style="5" bestFit="1" customWidth="1"/>
@@ -755,144 +772,155 @@
     <col min="14" max="14" width="21.08984375" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="25.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21.08984375" style="5" customWidth="1"/>
-    <col min="17" max="17" width="18.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.6328125" style="11" customWidth="1"/>
-    <col min="20" max="20" width="6.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7" style="5" customWidth="1"/>
-    <col min="29" max="30" width="12" style="5" customWidth="1"/>
-    <col min="31" max="31" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="24.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="8.7265625" style="5"/>
+    <col min="17" max="17" width="18" style="5" customWidth="1"/>
+    <col min="18" max="19" width="26.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.26953125" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.6328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.6328125" style="10" customWidth="1"/>
+    <col min="23" max="23" width="6.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" style="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7" style="5" customWidth="1"/>
+    <col min="32" max="33" width="12" style="5" customWidth="1"/>
+    <col min="34" max="34" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="X1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="U1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="AC1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>72</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AF1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>41</v>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C2" s="4">
         <v>1723</v>
@@ -904,96 +932,105 @@
         <v>11234846</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="T2" s="9">
+        <v>0</v>
+      </c>
+      <c r="U2" s="9">
         <v>3</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q2" s="10">
-        <v>0</v>
-      </c>
-      <c r="R2" s="10">
-        <v>3</v>
-      </c>
-      <c r="S2" s="10">
+      <c r="V2" s="9">
         <v>6</v>
       </c>
-      <c r="T2" s="10">
+      <c r="W2" s="9">
         <v>10</v>
       </c>
-      <c r="U2" s="10">
+      <c r="X2" s="9">
         <v>2001</v>
       </c>
-      <c r="V2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y2" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB2" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC2" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD2" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE2" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="AF2" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="AG2" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ2" s="3">
+      <c r="Y2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM2" s="3">
         <v>22</v>
       </c>
     </row>
@@ -1001,11 +1038,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J2:K2 AD2:AF2 AG2" numberStoredAsText="1"/>
+    <ignoredError sqref="J2:K2 AG2:AJ2 Q2:S2" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'-na-'!$C$2:$C$3</xm:f>
@@ -1032,16 +1069,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A1:AD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.453125" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.81640625" style="5" customWidth="1"/>
     <col min="5" max="5" width="19" style="5" customWidth="1"/>
@@ -1055,120 +1090,131 @@
     <col min="14" max="14" width="22.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="25.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="16.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.7265625" style="5"/>
-    <col min="27" max="27" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="8.7265625" style="5"/>
+    <col min="17" max="17" width="18" style="5" customWidth="1"/>
+    <col min="18" max="19" width="26.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="16.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.7265625" style="5"/>
+    <col min="30" max="30" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="X1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="U1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="AD1" s="1" t="s">
-        <v>41</v>
+        <v>63</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="C2" s="4">
         <v>1813</v>
@@ -1180,78 +1226,87 @@
         <v>11234846</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="J2" s="4">
         <v>13012004</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>83</v>
+      <c r="K2" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="P2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="T2" s="9">
+        <v>0</v>
+      </c>
+      <c r="U2" s="9">
+        <v>3</v>
+      </c>
+      <c r="V2" s="9">
+        <v>6</v>
+      </c>
+      <c r="W2" s="9">
+        <v>10</v>
+      </c>
+      <c r="X2" s="9">
+        <v>2001</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA2" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="Q2" s="10">
-        <v>0</v>
-      </c>
-      <c r="R2" s="10">
-        <v>3</v>
-      </c>
-      <c r="S2" s="10">
-        <v>6</v>
-      </c>
-      <c r="T2" s="10">
-        <v>10</v>
-      </c>
-      <c r="U2" s="10">
-        <v>2001</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y2" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD2" s="3">
+      <c r="AB2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG2" s="3">
         <v>22</v>
       </c>
     </row>
@@ -1259,7 +1314,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="Z2:AA2 K2" numberStoredAsText="1"/>
+    <ignoredError sqref="AC2:AD2 K2 Q2:S2" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1290,14 +1345,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.453125" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="19" style="5" bestFit="1" customWidth="1"/>
@@ -1313,129 +1368,140 @@
     <col min="17" max="17" width="19.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="25.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="16.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.7265625" style="5"/>
-    <col min="30" max="30" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="8.7265625" style="5"/>
+    <col min="20" max="20" width="18" style="5" customWidth="1"/>
+    <col min="21" max="22" width="26.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="16.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.7265625" style="5"/>
+    <col min="33" max="33" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="AA1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="X1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="AG1" s="1" t="s">
-        <v>41</v>
+        <v>63</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="C2" s="4">
         <v>1723</v>
@@ -1447,16 +1513,16 @@
         <v>20291427</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="J2" s="4">
         <v>2</v>
@@ -1467,67 +1533,76 @@
       <c r="L2" s="4">
         <v>1</v>
       </c>
-      <c r="M2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>84</v>
+      <c r="M2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="T2" s="10">
+        <v>55</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="W2" s="9">
         <v>0</v>
       </c>
-      <c r="U2" s="10">
+      <c r="X2" s="9">
         <v>3</v>
       </c>
-      <c r="V2" s="10">
+      <c r="Y2" s="9">
         <v>6</v>
       </c>
-      <c r="W2" s="10">
+      <c r="Z2" s="9">
         <v>10</v>
       </c>
-      <c r="X2" s="10">
+      <c r="AA2" s="9">
         <v>2001</v>
       </c>
-      <c r="Y2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB2" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC2" s="8" t="s">
+      <c r="AB2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD2" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="AD2" s="8" t="s">
+      <c r="AE2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG2" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="AE2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG2" s="3">
+      <c r="AH2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ2" s="3">
         <v>22</v>
       </c>
     </row>
@@ -1535,11 +1610,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="M2:N2 AC2:AD2" numberStoredAsText="1"/>
+    <ignoredError sqref="M2:N2 AF2:AG2 T2:V2" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'-na-'!$C$2:$C$3</xm:f>
@@ -1558,6 +1633,12 @@
           </x14:formula1>
           <xm:sqref>F2</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'-na-'!$F$2:$F$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:I2</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1568,8 +1649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1582,34 +1663,35 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>58</v>
+      <c r="A2" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1633,10 +1715,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F1" sqref="F1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1646,65 +1728,78 @@
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <v>1713</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3">
         <v>1723</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D4">
         <v>1813</v>
       </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D5">
         <v>1823</v>
       </c>

</xml_diff>

<commit_message>
partially updating actionitem_1 Entering 'First Maintenance' value if not available
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="98">
   <si>
     <t>A10137873</t>
   </si>
@@ -273,12 +273,6 @@
     <t>59.1</t>
   </si>
   <si>
-    <t>1f</t>
-  </si>
-  <si>
-    <t>95.48</t>
-  </si>
-  <si>
     <t>Sherbrooke</t>
   </si>
   <si>
@@ -292,9 +286,6 @@
   </si>
   <si>
     <t>AutomationCKQ</t>
-  </si>
-  <si>
-    <t>84.87</t>
   </si>
   <si>
     <t>isFirstMaintenancetoEdit</t>
@@ -846,13 +837,13 @@
         <v>54</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="T1" s="8" t="s">
         <v>17</v>
@@ -965,13 +956,13 @@
         <v>55</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="T2" s="9">
         <v>0</v>
@@ -1158,13 +1149,13 @@
         <v>54</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="T1" s="8" t="s">
         <v>17</v>
@@ -1214,7 +1205,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C2" s="4">
         <v>1813</v>
@@ -1259,13 +1250,13 @@
         <v>55</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="T2" s="9">
         <v>0</v>
@@ -1445,13 +1436,13 @@
         <v>54</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="W1" s="8" t="s">
         <v>17</v>
@@ -1501,7 +1492,7 @@
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C2" s="4">
         <v>1723</v>
@@ -1522,7 +1513,7 @@
         <v>46</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J2" s="4">
         <v>2</v>
@@ -1546,7 +1537,7 @@
         <v>57</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>53</v>
@@ -1555,13 +1546,13 @@
         <v>55</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="W2" s="9">
         <v>0</v>
@@ -1585,16 +1576,16 @@
         <v>64</v>
       </c>
       <c r="AD2" s="7" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="AE2" s="7" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="AF2" s="7" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="AG2" s="7" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="AH2" s="3" t="s">
         <v>40</v>
@@ -1610,7 +1601,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="M2:N2 AF2:AG2 T2:V2" numberStoredAsText="1"/>
+    <ignoredError sqref="M2:N2 T2:V2" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1748,7 +1739,7 @@
         <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1768,7 +1759,7 @@
         <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Grouping the test scripts based on manual test cases in robot and updating VerifyPriceCalculatedSuccessfully_TobecheckedinFrance due to application change in element location and row 9 10 11 12 field attribute changed from empty to zero in SBU_ROPES_BASE_NEW
</commit_message>
<xml_diff>
--- a/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
+++ b/KTOC_TRB_TestAutomation/TestData/KTOCTRB_AutomationTestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\con_svijay02\KTOC-TRB-Automation\KTOC_TRB_TestAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFA8451-4409-4BE0-B252-5FD09E7BFF2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="France" sheetId="7" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="76">
   <si>
     <t>A10137873</t>
   </si>
@@ -42,12 +43,6 @@
     <t>Supervisor</t>
   </si>
   <si>
-    <t>Discount</t>
-  </si>
-  <si>
-    <t>ITEfactor</t>
-  </si>
-  <si>
     <t>N194322</t>
   </si>
   <si>
@@ -81,21 +76,6 @@
     <t>TemplateName</t>
   </si>
   <si>
-    <t>withoutFirstMaintenance</t>
-  </si>
-  <si>
-    <t>withFirstMaintenance1</t>
-  </si>
-  <si>
-    <t>withFirstMaintenance2</t>
-  </si>
-  <si>
-    <t>TenderPrice</t>
-  </si>
-  <si>
-    <t>RegionalDiscount</t>
-  </si>
-  <si>
     <t>ios</t>
   </si>
   <si>
@@ -204,60 +184,18 @@
     <t>EIS Escalator</t>
   </si>
   <si>
-    <t>changeRegionalDiscount</t>
-  </si>
-  <si>
-    <t>changeITEfactor</t>
-  </si>
-  <si>
     <t>changeSupervisor</t>
   </si>
   <si>
     <t>06151495</t>
   </si>
   <si>
-    <t>LabourRate</t>
-  </si>
-  <si>
-    <t>changeLabourRate</t>
-  </si>
-  <si>
-    <t>0f</t>
-  </si>
-  <si>
-    <t>2.47f</t>
-  </si>
-  <si>
-    <t>73.68</t>
-  </si>
-  <si>
     <t>13010164</t>
   </si>
   <si>
     <t>07003009</t>
   </si>
   <si>
-    <t>RegionalDiscount_MultipleEqup</t>
-  </si>
-  <si>
-    <t>changeRegionalDiscount_MultipleEqup</t>
-  </si>
-  <si>
-    <t>ITEfactor_MultipleEqup</t>
-  </si>
-  <si>
-    <t>changeITEfactor_MultipleEqup</t>
-  </si>
-  <si>
-    <t>LabourRate_MultipleEqup</t>
-  </si>
-  <si>
-    <t>changeLabourRate__MultipleEqup</t>
-  </si>
-  <si>
-    <t>AUTOMATION TRB SFA</t>
-  </si>
-  <si>
     <t>s.vijay@kone.com.qap</t>
   </si>
   <si>
@@ -267,12 +205,6 @@
     <t>AutomationSFA</t>
   </si>
   <si>
-    <t>0.92f</t>
-  </si>
-  <si>
-    <t>59.1</t>
-  </si>
-  <si>
     <t>Sherbrooke</t>
   </si>
   <si>
@@ -322,12 +254,15 @@
   </si>
   <si>
     <t>185</t>
+  </si>
+  <si>
+    <t>AutomationKTOC SFA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -400,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -419,13 +354,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -740,8 +668,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -765,150 +693,83 @@
     <col min="16" max="16" width="21.08984375" style="5" customWidth="1"/>
     <col min="17" max="17" width="18" style="5" customWidth="1"/>
     <col min="18" max="19" width="26.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.26953125" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.6328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.6328125" style="10" customWidth="1"/>
-    <col min="23" max="23" width="6.81640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9" style="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7" style="5" customWidth="1"/>
-    <col min="32" max="33" width="12" style="5" customWidth="1"/>
-    <col min="34" max="34" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="8.7265625" style="5"/>
+    <col min="20" max="20" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="X1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>75</v>
@@ -923,7 +784,7 @@
         <v>11234846</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>0</v>
@@ -935,93 +796,42 @@
         <v>2</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="O2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="T2" s="9">
-        <v>0</v>
-      </c>
-      <c r="U2" s="9">
-        <v>3</v>
-      </c>
-      <c r="V2" s="9">
-        <v>6</v>
-      </c>
-      <c r="W2" s="9">
-        <v>10</v>
-      </c>
-      <c r="X2" s="9">
-        <v>2001</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AE2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG2" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH2" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="AI2" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="AJ2" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM2" s="3">
+        <v>70</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="3">
         <v>22</v>
       </c>
     </row>
@@ -1029,24 +839,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J2:K2 AG2:AJ2 Q2:S2" numberStoredAsText="1"/>
+    <ignoredError sqref="J2:K2 Q2:S2" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'-na-'!$C$2:$C$3</xm:f>
           </x14:formula1>
           <xm:sqref>A2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'-na-'!$D$2:$D$5</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>'-na-'!$E$2:$E$3</xm:f>
           </x14:formula1>
@@ -1059,8 +869,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1083,129 +893,86 @@
     <col min="16" max="16" width="17.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" style="5" customWidth="1"/>
     <col min="18" max="19" width="26.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="16.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.7265625" style="5"/>
-    <col min="30" max="30" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="8.7265625" style="5"/>
+    <col min="20" max="20" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="X1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="B2" s="4" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="C2" s="4">
         <v>1813</v>
@@ -1217,87 +984,54 @@
         <v>11234846</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J2" s="4">
         <v>13012004</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="T2" s="9">
-        <v>0</v>
-      </c>
-      <c r="U2" s="9">
-        <v>3</v>
-      </c>
-      <c r="V2" s="9">
-        <v>6</v>
-      </c>
-      <c r="W2" s="9">
-        <v>10</v>
-      </c>
-      <c r="X2" s="9">
-        <v>2001</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA2" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB2" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC2" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD2" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG2" s="3">
+        <v>73</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="3">
         <v>22</v>
       </c>
     </row>
@@ -1305,24 +1039,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="AC2:AD2 K2 Q2:S2" numberStoredAsText="1"/>
+    <ignoredError sqref="K2 Q2:S2" numberStoredAsText="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>'-na-'!$E$2:$E$3</xm:f>
           </x14:formula1>
           <xm:sqref>F2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>'-na-'!$D$2:$D$5</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>'-na-'!$C$2:$C$3</xm:f>
           </x14:formula1>
@@ -1335,8 +1069,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1361,138 +1095,95 @@
     <col min="19" max="19" width="17.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="18" style="5" customWidth="1"/>
     <col min="21" max="22" width="26.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="16.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.7265625" style="5"/>
-    <col min="33" max="33" width="13.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="8.7265625" style="5"/>
+    <col min="23" max="23" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" s="2" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="X1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="C2" s="4">
         <v>1723</v>
@@ -1504,16 +1195,16 @@
         <v>20291427</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="J2" s="4">
         <v>2</v>
@@ -1525,75 +1216,42 @@
         <v>1</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="W2" s="9">
-        <v>0</v>
-      </c>
-      <c r="X2" s="9">
-        <v>3</v>
-      </c>
-      <c r="Y2" s="9">
-        <v>6</v>
-      </c>
-      <c r="Z2" s="9">
-        <v>10</v>
-      </c>
-      <c r="AA2" s="9">
-        <v>2001</v>
-      </c>
-      <c r="AB2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ2" s="3">
+        <v>74</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y2" s="3">
         <v>22</v>
       </c>
     </row>
@@ -1606,25 +1264,25 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>'-na-'!$C$2:$C$3</xm:f>
           </x14:formula1>
           <xm:sqref>A2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>'-na-'!$D$2:$D$5</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
           <x14:formula1>
             <xm:f>'-na-'!$E$2:$E$3</xm:f>
           </x14:formula1>
           <xm:sqref>F2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000003000000}">
           <x14:formula1>
             <xm:f>'-na-'!$F$2:$F$4</xm:f>
           </x14:formula1>
@@ -1637,7 +1295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1654,30 +1312,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
-        <v>76</v>
+      <c r="A2" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1686,13 +1344,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>'-na-'!$B$2:$B$3</xm:f>
           </x14:formula1>
           <xm:sqref>D2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
             <xm:f>'-na-'!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -1705,7 +1363,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1724,62 +1382,62 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>1713</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>1723</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1787,7 +1445,7 @@
         <v>1813</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>